<commit_message>
Feat: 2 selection method comparison
</commit_message>
<xml_diff>
--- a/tp2/output/data/heatmap_avg.xlsx
+++ b/tp2/output/data/heatmap_avg.xlsx
@@ -38,110 +38,170 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="007A8400"/>
+        <bgColor rgb="007A8400"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00837B00"/>
+        <bgColor rgb="00837B00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0056A800"/>
+        <bgColor rgb="0056A800"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00758900"/>
+        <bgColor rgb="00758900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ED1100"/>
+        <bgColor rgb="00ED1100"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009C6200"/>
+        <bgColor rgb="009C6200"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004FAF00"/>
+        <bgColor rgb="004FAF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0030CE00"/>
+        <bgColor rgb="0030CE00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006D9100"/>
+        <bgColor rgb="006D9100"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0015E900"/>
+        <bgColor rgb="0015E900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0059A500"/>
+        <bgColor rgb="0059A500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F40A00"/>
+        <bgColor rgb="00F40A00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0053AB00"/>
+        <bgColor rgb="0053AB00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00689600"/>
+        <bgColor rgb="00689600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0028D600"/>
+        <bgColor rgb="0028D600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00778700"/>
+        <bgColor rgb="00778700"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00798500"/>
+        <bgColor rgb="00798500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0051AD00"/>
+        <bgColor rgb="0051AD00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CF2F00"/>
+        <bgColor rgb="00CF2F00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0020DE00"/>
+        <bgColor rgb="0020DE00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="0000FF00"/>
         <bgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="002ED000"/>
-        <bgColor rgb="002ED000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0035C900"/>
-        <bgColor rgb="0035C900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="006B9300"/>
         <bgColor rgb="006B9300"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0054AA00"/>
-        <bgColor rgb="0054AA00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00817D00"/>
-        <bgColor rgb="00817D00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0026D800"/>
-        <bgColor rgb="0026D800"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="007F7F00"/>
-        <bgColor rgb="007F7F00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="009A6400"/>
-        <bgColor rgb="009A6400"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D72700"/>
-        <bgColor rgb="00D72700"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00A85600"/>
-        <bgColor rgb="00A85600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00659900"/>
-        <bgColor rgb="00659900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="009F5F00"/>
-        <bgColor rgb="009F5F00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00946A00"/>
-        <bgColor rgb="00946A00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0024DA00"/>
-        <bgColor rgb="0024DA00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00778700"/>
-        <bgColor rgb="00778700"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="006F8F00"/>
-        <bgColor rgb="006F8F00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00728C00"/>
-        <bgColor rgb="00728C00"/>
+        <fgColor rgb="008B7300"/>
+        <bgColor rgb="008B7300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0010EE00"/>
+        <bgColor rgb="0010EE00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009E6000"/>
+        <bgColor rgb="009E6000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F20C00"/>
+        <bgColor rgb="00F20C00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A65800"/>
+        <bgColor rgb="00A65800"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009B6300"/>
+        <bgColor rgb="009B6300"/>
       </patternFill>
     </fill>
     <fill>
@@ -152,56 +212,80 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00906E00"/>
-        <bgColor rgb="00906E00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0055A900"/>
-        <bgColor rgb="0055A900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00609E00"/>
-        <bgColor rgb="00609E00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005EA000"/>
-        <bgColor rgb="005EA000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00976700"/>
-        <bgColor rgb="00976700"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00966800"/>
         <bgColor rgb="00966800"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F20C00"/>
-        <bgColor rgb="00F20C00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00768800"/>
-        <bgColor rgb="00768800"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E11D00"/>
-        <bgColor rgb="00E11D00"/>
+        <fgColor rgb="00DF1F00"/>
+        <bgColor rgb="00DF1F00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E31B00"/>
+        <bgColor rgb="00E31B00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CD3100"/>
+        <bgColor rgb="00CD3100"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00788600"/>
+        <bgColor rgb="00788600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0052AC00"/>
+        <bgColor rgb="0052AC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A95500"/>
+        <bgColor rgb="00A95500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FA0400"/>
+        <bgColor rgb="00FA0400"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005F9F00"/>
+        <bgColor rgb="005F9F00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00738B00"/>
+        <bgColor rgb="00738B00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004CB200"/>
+        <bgColor rgb="004CB200"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FE00"/>
+        <bgColor rgb="0000FE00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00936B00"/>
+        <bgColor rgb="00936B00"/>
       </patternFill>
     </fill>
     <fill>
@@ -212,98 +296,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00A55900"/>
-        <bgColor rgb="00A55900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FB0300"/>
-        <bgColor rgb="00FB0300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E21C00"/>
-        <bgColor rgb="00E21C00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00A95500"/>
-        <bgColor rgb="00A95500"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="008A7400"/>
-        <bgColor rgb="008A7400"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E81600"/>
-        <bgColor rgb="00E81600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00996500"/>
-        <bgColor rgb="00996500"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00B14D00"/>
-        <bgColor rgb="00B14D00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C83600"/>
-        <bgColor rgb="00C83600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00B24C00"/>
-        <bgColor rgb="00B24C00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CD3100"/>
-        <bgColor rgb="00CD3100"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00DE2000"/>
-        <bgColor rgb="00DE2000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CF2F00"/>
-        <bgColor rgb="00CF2F00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00EE1000"/>
-        <bgColor rgb="00EE1000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D52900"/>
-        <bgColor rgb="00D52900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00B34B00"/>
-        <bgColor rgb="00B34B00"/>
+        <fgColor rgb="00AF4F00"/>
+        <bgColor rgb="00AF4F00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005AA400"/>
+        <bgColor rgb="005AA400"/>
       </patternFill>
     </fill>
   </fills>
@@ -797,25 +797,25 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>21.49827450647811</v>
+        <v>34.56961047698816</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>19.87476059622278</v>
+        <v>33.80734890733969</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>19.63934263178244</v>
+        <v>37.4009995487917</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>17.78056347189124</v>
+        <v>34.91749846749504</v>
       </c>
       <c r="F2" s="6" t="n">
-        <v>18.55675234869073</v>
+        <v>25.34509611142192</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>17.01597873923405</v>
+        <v>31.7990593904367</v>
       </c>
       <c r="H2" s="8" t="n">
-        <v>20.16196224399202</v>
+        <v>37.97430692586236</v>
       </c>
     </row>
     <row r="3">
@@ -825,25 +825,25 @@
         </is>
       </c>
       <c r="B3" s="9" t="n">
-        <v>17.07163775091502</v>
+        <v>40.47327286965997</v>
       </c>
       <c r="C3" s="10" t="n">
-        <v>16.124652958309</v>
+        <v>35.53855625658157</v>
       </c>
       <c r="D3" s="11" t="n">
-        <v>14.01000420150013</v>
+        <v>42.6031532407655</v>
       </c>
       <c r="E3" s="12" t="n">
-        <v>15.66716409801395</v>
+        <v>37.19251862144604</v>
       </c>
       <c r="F3" s="13" t="n">
-        <v>17.98876589979829</v>
+        <v>24.75561981086007</v>
       </c>
       <c r="G3" s="14" t="n">
-        <v>15.97221872840986</v>
+        <v>37.67543018932605</v>
       </c>
       <c r="H3" s="15" t="n">
-        <v>16.35460590536126</v>
+        <v>35.98653271380643</v>
       </c>
     </row>
     <row r="4">
@@ -853,25 +853,25 @@
         </is>
       </c>
       <c r="B4" s="16" t="n">
-        <v>20.22020236506072</v>
+        <v>41.09484843297938</v>
       </c>
       <c r="C4" s="17" t="n">
-        <v>17.35298773499225</v>
+        <v>34.79410437901196</v>
       </c>
       <c r="D4" s="18" t="n">
-        <v>17.64102339244477</v>
+        <v>34.59453478003564</v>
       </c>
       <c r="E4" s="19" t="n">
-        <v>17.51859735976329</v>
+        <v>37.80605058970866</v>
       </c>
       <c r="F4" s="20" t="n">
-        <v>19.4959983962142</v>
+        <v>27.75370273939263</v>
       </c>
       <c r="G4" s="21" t="n">
-        <v>16.47232700157192</v>
+        <v>41.71637599345106</v>
       </c>
       <c r="H4" s="22" t="n">
-        <v>18.52773786189685</v>
+        <v>44.34695207176806</v>
       </c>
     </row>
     <row r="5">
@@ -881,25 +881,25 @@
         </is>
       </c>
       <c r="B5" s="23" t="n">
-        <v>18.1638095386172</v>
+        <v>35.75844205240179</v>
       </c>
       <c r="C5" s="24" t="n">
-        <v>18.2179066990033</v>
+        <v>33.13156521967881</v>
       </c>
       <c r="D5" s="25" t="n">
-        <v>16.25868327395341</v>
+        <v>43.0640543929394</v>
       </c>
       <c r="E5" s="26" t="n">
-        <v>16.27296090215496</v>
+        <v>31.6862663422086</v>
       </c>
       <c r="F5" s="27" t="n">
-        <v>13.10299842009066</v>
+        <v>24.91005816390107</v>
       </c>
       <c r="G5" s="28" t="n">
-        <v>17.37558697931734</v>
-      </c>
-      <c r="H5" s="29" t="n">
-        <v>13.69536214820151</v>
+        <v>31.01223338395964</v>
+      </c>
+      <c r="H5" s="18" t="n">
+        <v>34.61759678191667</v>
       </c>
     </row>
     <row r="6">
@@ -908,26 +908,26 @@
           <t>ranking</t>
         </is>
       </c>
-      <c r="B6" s="30" t="n">
-        <v>12.65766482454001</v>
-      </c>
-      <c r="C6" s="31" t="n">
-        <v>15.74345965752987</v>
-      </c>
-      <c r="D6" s="32" t="n">
-        <v>12.77567745284902</v>
-      </c>
-      <c r="E6" s="33" t="n">
-        <v>13.64810496553802</v>
-      </c>
-      <c r="F6" s="34" t="n">
-        <v>15.62572391636405</v>
-      </c>
-      <c r="G6" s="35" t="n">
-        <v>16.69623044332418</v>
-      </c>
-      <c r="H6" s="36" t="n">
-        <v>13.44155023971269</v>
+      <c r="B6" s="29" t="n">
+        <v>31.90840413364006</v>
+      </c>
+      <c r="C6" s="30" t="n">
+        <v>39.72221773918098</v>
+      </c>
+      <c r="D6" s="31" t="n">
+        <v>32.31729905358404</v>
+      </c>
+      <c r="E6" s="20" t="n">
+        <v>27.74017232498452</v>
+      </c>
+      <c r="F6" s="32" t="n">
+        <v>26.41968659287506</v>
+      </c>
+      <c r="G6" s="33" t="n">
+        <v>26.14021771976047</v>
+      </c>
+      <c r="H6" s="34" t="n">
+        <v>27.84719073469019</v>
       </c>
     </row>
     <row r="7">
@@ -936,26 +936,26 @@
           <t>roulette</t>
         </is>
       </c>
-      <c r="B7" s="37" t="n">
-        <v>16.18682524919912</v>
-      </c>
-      <c r="C7" s="26" t="n">
-        <v>16.29368480817576</v>
-      </c>
-      <c r="D7" s="38" t="n">
-        <v>15.34946580081668</v>
-      </c>
-      <c r="E7" s="39" t="n">
-        <v>14.56007519607936</v>
-      </c>
-      <c r="F7" s="40" t="n">
-        <v>15.30617729791973</v>
-      </c>
-      <c r="G7" s="41" t="n">
-        <v>14.3779016596445</v>
-      </c>
-      <c r="H7" s="19" t="n">
-        <v>17.53575565764529</v>
+      <c r="B7" s="35" t="n">
+        <v>34.71321406236066</v>
+      </c>
+      <c r="C7" s="18" t="n">
+        <v>34.63919572821099</v>
+      </c>
+      <c r="D7" s="36" t="n">
+        <v>37.72031811324442</v>
+      </c>
+      <c r="E7" s="37" t="n">
+        <v>30.77603239243721</v>
+      </c>
+      <c r="F7" s="38" t="n">
+        <v>24.24797968996332</v>
+      </c>
+      <c r="G7" s="7" t="n">
+        <v>31.78380278526826</v>
+      </c>
+      <c r="H7" s="39" t="n">
+        <v>36.73144205872207</v>
       </c>
     </row>
     <row r="8">
@@ -964,26 +964,26 @@
           <t>universal</t>
         </is>
       </c>
-      <c r="B8" s="24" t="n">
-        <v>18.23867112811237</v>
-      </c>
-      <c r="C8" s="42" t="n">
-        <v>13.78027412486982</v>
-      </c>
-      <c r="D8" s="43" t="n">
-        <v>14.30065888223345</v>
-      </c>
-      <c r="E8" s="44" t="n">
-        <v>13.24455882203625</v>
-      </c>
-      <c r="F8" s="45" t="n">
-        <v>14.10261397963126</v>
-      </c>
-      <c r="G8" s="40" t="n">
-        <v>15.32355745118401</v>
+      <c r="B8" s="40" t="n">
+        <v>35.07816453210451</v>
+      </c>
+      <c r="C8" s="41" t="n">
+        <v>38.25313599468108</v>
+      </c>
+      <c r="D8" s="42" t="n">
+        <v>44.2939803401427</v>
+      </c>
+      <c r="E8" s="43" t="n">
+        <v>32.52113367125919</v>
+      </c>
+      <c r="F8" s="44" t="n">
+        <v>23.91484095570765</v>
+      </c>
+      <c r="G8" s="45" t="n">
+        <v>30.31629387995409</v>
       </c>
       <c r="H8" s="46" t="n">
-        <v>15.28824107963455</v>
+        <v>37.07141533528127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat: selection rate analysis
</commit_message>
<xml_diff>
--- a/tp2/output/data/heatmap_avg.xlsx
+++ b/tp2/output/data/heatmap_avg.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="47">
+  <fills count="45">
     <fill>
       <patternFill/>
     </fill>
@@ -38,44 +38,212 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="007A8400"/>
-        <bgColor rgb="007A8400"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00837B00"/>
-        <bgColor rgb="00837B00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0056A800"/>
-        <bgColor rgb="0056A800"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00758900"/>
-        <bgColor rgb="00758900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ED1100"/>
-        <bgColor rgb="00ED1100"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="009C6200"/>
-        <bgColor rgb="009C6200"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004FAF00"/>
-        <bgColor rgb="004FAF00"/>
+        <fgColor rgb="0028D600"/>
+        <bgColor rgb="0028D600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003DC100"/>
+        <bgColor rgb="003DC100"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0005F900"/>
+        <bgColor rgb="0005F900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="001AE400"/>
+        <bgColor rgb="001AE400"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0047B700"/>
+        <bgColor rgb="0047B700"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000DF100"/>
+        <bgColor rgb="000DF100"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0038C600"/>
+        <bgColor rgb="0038C600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0011ED00"/>
+        <bgColor rgb="0011ED00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0009F500"/>
+        <bgColor rgb="0009F500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0006F800"/>
+        <bgColor rgb="0006F800"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002AD400"/>
+        <bgColor rgb="002AD400"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0016E800"/>
+        <bgColor rgb="0016E800"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0004FA00"/>
+        <bgColor rgb="0004FA00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0013EB00"/>
+        <bgColor rgb="0013EB00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0019E500"/>
+        <bgColor rgb="0019E500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0017E700"/>
+        <bgColor rgb="0017E700"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000BF300"/>
+        <bgColor rgb="000BF300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0033CB00"/>
+        <bgColor rgb="0033CB00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00679700"/>
+        <bgColor rgb="00679700"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="007C8200"/>
+        <bgColor rgb="007C8200"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00BC4200"/>
+        <bgColor rgb="00BC4200"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FC0200"/>
+        <bgColor rgb="00FC0200"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C43A00"/>
+        <bgColor rgb="00C43A00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CD3100"/>
+        <bgColor rgb="00CD3100"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FE0000"/>
+        <bgColor rgb="00FE0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E61800"/>
+        <bgColor rgb="00E61800"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EB1300"/>
+        <bgColor rgb="00EB1300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E51900"/>
+        <bgColor rgb="00E51900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0041BD00"/>
+        <bgColor rgb="0041BD00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0029D500"/>
+        <bgColor rgb="0029D500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="001DE100"/>
+        <bgColor rgb="001DE100"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0040BE00"/>
+        <bgColor rgb="0040BE00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00877700"/>
+        <bgColor rgb="00877700"/>
       </patternFill>
     </fill>
     <fill>
@@ -86,224 +254,44 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="006D9100"/>
-        <bgColor rgb="006D9100"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="0015E900"/>
         <bgColor rgb="0015E900"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0059A500"/>
-        <bgColor rgb="0059A500"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F40A00"/>
-        <bgColor rgb="00F40A00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0053AB00"/>
-        <bgColor rgb="0053AB00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00689600"/>
-        <bgColor rgb="00689600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0028D600"/>
-        <bgColor rgb="0028D600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00778700"/>
-        <bgColor rgb="00778700"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00798500"/>
-        <bgColor rgb="00798500"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0051AD00"/>
-        <bgColor rgb="0051AD00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CF2F00"/>
-        <bgColor rgb="00CF2F00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0020DE00"/>
-        <bgColor rgb="0020DE00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0000FF00"/>
-        <bgColor rgb="0000FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="006B9300"/>
-        <bgColor rgb="006B9300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="008B7300"/>
-        <bgColor rgb="008B7300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0010EE00"/>
-        <bgColor rgb="0010EE00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="009E6000"/>
-        <bgColor rgb="009E6000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F20C00"/>
-        <bgColor rgb="00F20C00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00A65800"/>
-        <bgColor rgb="00A65800"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="009B6300"/>
-        <bgColor rgb="009B6300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0039C500"/>
-        <bgColor rgb="0039C500"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00966800"/>
-        <bgColor rgb="00966800"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00DF1F00"/>
-        <bgColor rgb="00DF1F00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E31B00"/>
-        <bgColor rgb="00E31B00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CD3100"/>
-        <bgColor rgb="00CD3100"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00788600"/>
-        <bgColor rgb="00788600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0052AC00"/>
-        <bgColor rgb="0052AC00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00A95500"/>
-        <bgColor rgb="00A95500"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FA0400"/>
-        <bgColor rgb="00FA0400"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005F9F00"/>
-        <bgColor rgb="005F9F00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00738B00"/>
-        <bgColor rgb="00738B00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004CB200"/>
-        <bgColor rgb="004CB200"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0000FE00"/>
-        <bgColor rgb="0000FE00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00936B00"/>
-        <bgColor rgb="00936B00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00AF4F00"/>
-        <bgColor rgb="00AF4F00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005AA400"/>
-        <bgColor rgb="005AA400"/>
+        <fgColor rgb="0012EC00"/>
+        <bgColor rgb="0012EC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000EF000"/>
+        <bgColor rgb="000EF000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003FBF00"/>
+        <bgColor rgb="003FBF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0042BC00"/>
+        <bgColor rgb="0042BC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0014EA00"/>
+        <bgColor rgb="0014EA00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0024DA00"/>
+        <bgColor rgb="0024DA00"/>
       </patternFill>
     </fill>
   </fills>
@@ -325,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -373,8 +361,6 @@
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -797,25 +783,25 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>34.56961047698816</v>
+        <v>50.20042370379998</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>33.80734890733969</v>
+        <v>45.27175804369728</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>37.4009995487917</v>
+        <v>58.22726894608637</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>34.91749846749504</v>
+        <v>53.28008276277124</v>
       </c>
       <c r="F2" s="6" t="n">
-        <v>25.34509611142192</v>
+        <v>42.9607013789067</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>31.7990593904367</v>
+        <v>56.41630709397024</v>
       </c>
       <c r="H2" s="8" t="n">
-        <v>37.97430692586236</v>
+        <v>46.32124325804784</v>
       </c>
     </row>
     <row r="3">
@@ -825,25 +811,25 @@
         </is>
       </c>
       <c r="B3" s="9" t="n">
-        <v>40.47327286965997</v>
+        <v>55.49720409359161</v>
       </c>
       <c r="C3" s="10" t="n">
-        <v>35.53855625658157</v>
+        <v>57.45705811826789</v>
       </c>
       <c r="D3" s="11" t="n">
-        <v>42.6031532407655</v>
+        <v>58.08709984600456</v>
       </c>
       <c r="E3" s="12" t="n">
-        <v>37.19251862144604</v>
+        <v>59.5781144390805</v>
       </c>
       <c r="F3" s="13" t="n">
-        <v>24.75561981086007</v>
-      </c>
-      <c r="G3" s="14" t="n">
-        <v>37.67543018932605</v>
-      </c>
-      <c r="H3" s="15" t="n">
-        <v>35.98653271380643</v>
+        <v>49.58631285825091</v>
+      </c>
+      <c r="G3" s="10" t="n">
+        <v>57.32189727833821</v>
+      </c>
+      <c r="H3" s="14" t="n">
+        <v>54.21890231373295</v>
       </c>
     </row>
     <row r="4">
@@ -852,26 +838,26 @@
           <t>elite</t>
         </is>
       </c>
-      <c r="B4" s="16" t="n">
-        <v>41.09484843297938</v>
-      </c>
-      <c r="C4" s="17" t="n">
-        <v>34.79410437901196</v>
-      </c>
-      <c r="D4" s="18" t="n">
-        <v>34.59453478003564</v>
-      </c>
-      <c r="E4" s="19" t="n">
-        <v>37.80605058970866</v>
-      </c>
-      <c r="F4" s="20" t="n">
-        <v>27.75370273939263</v>
-      </c>
-      <c r="G4" s="21" t="n">
-        <v>41.71637599345106</v>
-      </c>
-      <c r="H4" s="22" t="n">
-        <v>44.34695207176806</v>
+      <c r="B4" s="15" t="n">
+        <v>58.63175040501206</v>
+      </c>
+      <c r="C4" s="16" t="n">
+        <v>54.99362814496135</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>58.20364465853443</v>
+      </c>
+      <c r="E4" s="17" t="n">
+        <v>53.63340434759237</v>
+      </c>
+      <c r="F4" s="18" t="n">
+        <v>54.16663365340688</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>58.33616829148674</v>
+      </c>
+      <c r="H4" s="19" t="n">
+        <v>56.99101942807872</v>
       </c>
     </row>
     <row r="5">
@@ -880,26 +866,26 @@
           <t>probabilistic_tournament</t>
         </is>
       </c>
-      <c r="B5" s="23" t="n">
-        <v>35.75844205240179</v>
-      </c>
-      <c r="C5" s="24" t="n">
-        <v>33.13156521967881</v>
-      </c>
-      <c r="D5" s="25" t="n">
-        <v>43.0640543929394</v>
-      </c>
-      <c r="E5" s="26" t="n">
-        <v>31.6862663422086</v>
-      </c>
-      <c r="F5" s="27" t="n">
-        <v>24.91005816390107</v>
-      </c>
-      <c r="G5" s="28" t="n">
-        <v>31.01223338395964</v>
-      </c>
-      <c r="H5" s="18" t="n">
-        <v>34.61759678191667</v>
+      <c r="B5" s="20" t="n">
+        <v>47.48398458751824</v>
+      </c>
+      <c r="C5" s="21" t="n">
+        <v>35.45027347797769</v>
+      </c>
+      <c r="D5" s="22" t="n">
+        <v>30.51979929405618</v>
+      </c>
+      <c r="E5" s="23" t="n">
+        <v>15.60136720128476</v>
+      </c>
+      <c r="F5" s="24" t="n">
+        <v>0.4698171143231041</v>
+      </c>
+      <c r="G5" s="25" t="n">
+        <v>13.6305712047328</v>
+      </c>
+      <c r="H5" s="26" t="n">
+        <v>11.58444127509778</v>
       </c>
     </row>
     <row r="6">
@@ -908,26 +894,26 @@
           <t>ranking</t>
         </is>
       </c>
-      <c r="B6" s="29" t="n">
-        <v>31.90840413364006</v>
-      </c>
-      <c r="C6" s="30" t="n">
-        <v>39.72221773918098</v>
-      </c>
-      <c r="D6" s="31" t="n">
-        <v>32.31729905358404</v>
-      </c>
-      <c r="E6" s="20" t="n">
-        <v>27.74017232498452</v>
-      </c>
-      <c r="F6" s="32" t="n">
-        <v>26.41968659287506</v>
-      </c>
-      <c r="G6" s="33" t="n">
-        <v>26.14021771976047</v>
-      </c>
-      <c r="H6" s="34" t="n">
-        <v>27.84719073469019</v>
+      <c r="B6" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="28" t="n">
+        <v>0.07432891683710323</v>
+      </c>
+      <c r="D6" s="29" t="n">
+        <v>5.648643550309048</v>
+      </c>
+      <c r="E6" s="28" t="n">
+        <v>0.1601679379734482</v>
+      </c>
+      <c r="F6" s="28" t="n">
+        <v>0.0701138574633708</v>
+      </c>
+      <c r="G6" s="30" t="n">
+        <v>4.640320631686636</v>
+      </c>
+      <c r="H6" s="31" t="n">
+        <v>5.867584428199558</v>
       </c>
     </row>
     <row r="7">
@@ -936,26 +922,26 @@
           <t>roulette</t>
         </is>
       </c>
-      <c r="B7" s="35" t="n">
-        <v>34.71321406236066</v>
-      </c>
-      <c r="C7" s="18" t="n">
-        <v>34.63919572821099</v>
-      </c>
-      <c r="D7" s="36" t="n">
-        <v>37.72031811324442</v>
-      </c>
-      <c r="E7" s="37" t="n">
-        <v>30.77603239243721</v>
-      </c>
-      <c r="F7" s="38" t="n">
-        <v>24.24797968996332</v>
-      </c>
-      <c r="G7" s="7" t="n">
-        <v>31.78380278526826</v>
-      </c>
-      <c r="H7" s="39" t="n">
-        <v>36.73144205872207</v>
+      <c r="B7" s="32" t="n">
+        <v>44.24702509430013</v>
+      </c>
+      <c r="C7" s="33" t="n">
+        <v>49.85025736673514</v>
+      </c>
+      <c r="D7" s="34" t="n">
+        <v>52.58254957361095</v>
+      </c>
+      <c r="E7" s="35" t="n">
+        <v>44.39212342534687</v>
+      </c>
+      <c r="F7" s="36" t="n">
+        <v>27.84715020426879</v>
+      </c>
+      <c r="G7" s="37" t="n">
+        <v>48.18677941681856</v>
+      </c>
+      <c r="H7" s="38" t="n">
+        <v>54.45795137122398</v>
       </c>
     </row>
     <row r="8">
@@ -964,26 +950,26 @@
           <t>universal</t>
         </is>
       </c>
-      <c r="B8" s="40" t="n">
-        <v>35.07816453210451</v>
-      </c>
-      <c r="C8" s="41" t="n">
-        <v>38.25313599468108</v>
-      </c>
-      <c r="D8" s="42" t="n">
-        <v>44.2939803401427</v>
-      </c>
-      <c r="E8" s="43" t="n">
-        <v>32.52113367125919</v>
-      </c>
-      <c r="F8" s="44" t="n">
-        <v>23.91484095570765</v>
-      </c>
-      <c r="G8" s="45" t="n">
-        <v>30.31629387995409</v>
-      </c>
-      <c r="H8" s="46" t="n">
-        <v>37.07141533528127</v>
+      <c r="B8" s="39" t="n">
+        <v>55.19924749119318</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>56.31386369036295</v>
+      </c>
+      <c r="D8" s="40" t="n">
+        <v>56.24083834680308</v>
+      </c>
+      <c r="E8" s="41" t="n">
+        <v>44.76401167907224</v>
+      </c>
+      <c r="F8" s="42" t="n">
+        <v>43.94959671754804</v>
+      </c>
+      <c r="G8" s="43" t="n">
+        <v>54.84820499745327</v>
+      </c>
+      <c r="H8" s="44" t="n">
+        <v>51.10474368228028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>